<commit_message>
delete drivers on recreation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="league" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="League" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Liveries" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -119,204 +119,204 @@
     <t xml:space="preserve">Barichello</t>
   </si>
   <si>
+    <t xml:space="preserve">Porsche GT3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G Racing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jarno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trulli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bentley 2020 GT3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eddie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irvine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porsche GT3 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luciano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">McLaren 650s GT3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaguar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herbert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">McLaren 650s GT3 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ralf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schmumacher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMW M6 GT3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jenson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMW M6 GT3 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giancarlo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fisichella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMW M4 GT3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benetton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aelxander</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wurz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMW M4 GT3 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audi GT3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heidfeld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audi GT3 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diniz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corvette GT3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sauber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corvette GT3 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de la Rosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radical GT3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verstappen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radical GT3 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">McLaren 720 S GT3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minardi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mazzacane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">McLaren 720 S GT3 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaccques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vilneuve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aston Martin GT3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ricardo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zonta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aston Martin GT3 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dominik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaetuso</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ferrari 488 GT3 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Jarno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trulli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bentley 2020 GT3 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jordan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eddie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Irvine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porsche GT3 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G-Point Racing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luciano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">McLaren 650s GT3 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jaguar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jonny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herbert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">McLaren 650s GT3 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ralf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schmumacher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMW M6 GT3 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jenson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMW M6 GT3 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giancarlo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fisichella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMW M4 GT3 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benetton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aelxander</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wurz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMW M4 GT3 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alesi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audi GT3 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heidfeld</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audi GT3 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diniz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corvette GT3 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sauber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corvette GT3 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de la Rosa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radical GT3 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arrows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verstappen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radical GT3 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">McLaren 720 S GT3 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minardi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaston</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazzacane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">McLaren 720 S GT3 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jaccques</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vilneuve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aston Martin GT3 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ricardo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zonta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aston Martin GT3 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dominik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaetuso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porsche GT3 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Heinz-Harald</t>
   </si>
   <si>
@@ -329,10 +329,10 @@
     <t xml:space="preserve">Livery Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Veh File</t>
+    <t xml:space="preserve">folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">veh_file</t>
   </si>
   <si>
     <t xml:space="preserve">Ferrari_488_GT3_2020</t>
@@ -484,6 +484,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -491,14 +497,8 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,6 +521,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFAFAFA"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFAFAFA"/>
       </patternFill>
     </fill>
     <fill>
@@ -564,7 +570,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -581,7 +587,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -589,19 +595,43 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -634,7 +664,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFAFAFA"/>
+      <rgbColor rgb="FFFFFFD7"/>
       <rgbColor rgb="FFF3F3F3"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -649,7 +679,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFFAFAFA"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
@@ -682,10 +712,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:XFD25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -709,8 +739,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16380" min="16380" style="0" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="1" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16380" style="1" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -802,7 +831,7 @@
         <v>100</v>
       </c>
       <c r="J2" s="3" t="n">
-        <f aca="false">league!$H4</f>
+        <f aca="false">League!$H4</f>
         <v>95</v>
       </c>
       <c r="K2" s="3" t="n">
@@ -812,14 +841,13 @@
         <v>73</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="N2" s="3" t="n">
         <v>97</v>
       </c>
       <c r="O2" s="3" t="n">
-        <f aca="false">ROUND(league!$H4*0.5, 0)</f>
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="P2" s="3" t="n">
         <v>100</v>
@@ -864,8 +892,8 @@
         <v>100</v>
       </c>
       <c r="J3" s="5" t="n">
-        <f aca="false">league!$H20</f>
-        <v>94</v>
+        <f aca="false">League!$H20</f>
+        <v>40</v>
       </c>
       <c r="K3" s="5" t="n">
         <v>10</v>
@@ -874,14 +902,13 @@
         <v>69</v>
       </c>
       <c r="M3" s="5" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="N3" s="5" t="n">
         <v>95</v>
       </c>
       <c r="O3" s="5" t="n">
-        <f aca="false">ROUND(league!$H20*0.5, 0)</f>
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="P3" s="5" t="n">
         <v>100</v>
@@ -935,17 +962,16 @@
         <v>89</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="N4" s="3" t="n">
         <v>94</v>
       </c>
       <c r="O4" s="3" t="n">
-        <f aca="false">ROUND(league!$H6*0.5, 0)</f>
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="P4" s="3" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Q4" s="3" t="n">
         <v>80</v>
@@ -974,21 +1000,21 @@
       <c r="E5" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>22</v>
+      <c r="G5" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>95</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J5" s="5" t="n">
-        <f aca="false">league!$H14</f>
-        <v>91</v>
+        <f aca="false">League!$H14</f>
+        <v>68</v>
       </c>
       <c r="K5" s="5" t="n">
         <v>50</v>
@@ -997,17 +1023,16 @@
         <v>84</v>
       </c>
       <c r="M5" s="5" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="N5" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="O5" s="5" t="n">
-        <f aca="false">ROUND(league!$H14*0.5, 0)</f>
-        <v>46</v>
+      <c r="O5" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="P5" s="5" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Q5" s="5" t="n">
         <v>80</v>
@@ -1021,10 +1046,10 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3" t="str">
         <f aca="false">A6&amp;" "&amp;B6</f>
@@ -1036,20 +1061,20 @@
       <c r="E6" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>35</v>
+      <c r="F6" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H6" s="3" t="n">
         <v>90</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J6" s="3" t="n">
-        <f aca="false">league!$H3</f>
+        <f aca="false">League!$H3</f>
         <v>100</v>
       </c>
       <c r="K6" s="3" t="n">
@@ -1059,17 +1084,16 @@
         <v>86</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="N6" s="3" t="n">
         <v>99</v>
       </c>
       <c r="O6" s="3" t="n">
-        <f aca="false">ROUND(league!$H3*0.5, 0)</f>
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="P6" s="3" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q6" s="3" t="n">
         <v>80</v>
@@ -1083,10 +1107,10 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="5" t="str">
         <f aca="false">A7&amp;" "&amp;B7</f>
@@ -1099,19 +1123,19 @@
         <v>6</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>90</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J7" s="5" t="n">
-        <f aca="false">league!$H12</f>
+        <f aca="false">League!$H12</f>
         <v>92</v>
       </c>
       <c r="K7" s="5" t="n">
@@ -1121,17 +1145,16 @@
         <v>71</v>
       </c>
       <c r="M7" s="5" t="n">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="N7" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="O7" s="5" t="n">
-        <f aca="false">ROUND(league!$H12*0.5, 0)</f>
-        <v>46</v>
+      <c r="O7" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="P7" s="5" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q7" s="5" t="n">
         <v>80</v>
@@ -1160,20 +1183,20 @@
       <c r="E8" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>44</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J8" s="3" t="n">
-        <f aca="false">league!$H5</f>
+        <f aca="false">League!$H5</f>
         <v>95</v>
       </c>
       <c r="K8" s="3" t="n">
@@ -1189,11 +1212,10 @@
         <v>100</v>
       </c>
       <c r="O8" s="3" t="n">
-        <f aca="false">ROUND(league!$H5*0.5, 0)</f>
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="P8" s="3" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q8" s="3" t="n">
         <v>80</v>
@@ -1205,67 +1227,71 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+    <row r="9" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="5" t="str">
+      <c r="C9" s="8" t="str">
         <f aca="false">A9&amp;" "&amp;B9</f>
         <v>Jonny Herbert</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="3" t="n">
-        <v>93</v>
+      <c r="H9" s="8" t="n">
+        <v>30</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="J9" s="5" t="n">
-        <f aca="false">league!$H13</f>
-        <v>90</v>
-      </c>
-      <c r="K9" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="J9" s="8" t="n">
+        <f aca="false">League!$H13</f>
+        <v>20</v>
+      </c>
+      <c r="K9" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="L9" s="5" t="n">
+      <c r="L9" s="8" t="n">
         <v>86</v>
       </c>
-      <c r="M9" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="N9" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="O9" s="5" t="n">
-        <f aca="false">ROUND(league!$H13*0.5, 0)</f>
-        <v>45</v>
+      <c r="M9" s="8" t="n">
+        <v>50</v>
+      </c>
+      <c r="N9" s="8" t="n">
+        <v>100</v>
+      </c>
+      <c r="O9" s="8" t="n">
+        <v>30</v>
       </c>
       <c r="P9" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q9" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="R9" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="S9" s="5" t="n">
-        <v>80</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="Q9" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="R9" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="S9" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="XEZ9" s="11"/>
+      <c r="XFA9" s="11"/>
+      <c r="XFB9" s="11"/>
+      <c r="XFC9" s="11"/>
+      <c r="XFD9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
@@ -1291,13 +1317,13 @@
         <v>51</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J10" s="3" t="n">
-        <f aca="false">league!$H7</f>
+        <f aca="false">League!$H7</f>
         <v>90</v>
       </c>
       <c r="K10" s="3" t="n">
@@ -1313,11 +1339,10 @@
         <v>100</v>
       </c>
       <c r="O10" s="3" t="n">
-        <f aca="false">ROUND(league!$H7*0.5, 0)</f>
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="P10" s="3" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q10" s="3" t="n">
         <v>80</v>
@@ -1353,14 +1378,14 @@
         <v>51</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J11" s="5" t="n">
-        <f aca="false">league!$H21</f>
-        <v>92</v>
+        <f aca="false">League!$H21</f>
+        <v>74</v>
       </c>
       <c r="K11" s="5" t="n">
         <v>23</v>
@@ -1374,12 +1399,11 @@
       <c r="N11" s="5" t="n">
         <v>92</v>
       </c>
-      <c r="O11" s="5" t="n">
-        <f aca="false">ROUND(league!$H21*0.5, 0)</f>
-        <v>46</v>
+      <c r="O11" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="P11" s="5" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q11" s="5" t="n">
         <v>80</v>
@@ -1418,11 +1442,11 @@
         <v>92</v>
       </c>
       <c r="I12" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J12" s="3" t="n">
-        <f aca="false">league!$H18</f>
-        <v>93</v>
+        <f aca="false">League!$H18</f>
+        <v>58</v>
       </c>
       <c r="K12" s="3" t="n">
         <v>54</v>
@@ -1437,11 +1461,10 @@
         <v>92</v>
       </c>
       <c r="O12" s="3" t="n">
-        <f aca="false">ROUND(league!$H18*0.5, 0)</f>
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="P12" s="3" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q12" s="3" t="n">
         <v>80</v>
@@ -1453,67 +1476,71 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+    <row r="13" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="5" t="str">
+      <c r="C13" s="8" t="str">
         <f aca="false">A13&amp;" "&amp;B13</f>
         <v>Aelxander Wurz</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H13" s="3" t="n">
+      <c r="H13" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="I13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="J13" s="8" t="n">
+        <f aca="false">League!$H19</f>
         <v>90</v>
       </c>
-      <c r="I13" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="J13" s="5" t="n">
-        <f aca="false">league!$H19</f>
-        <v>90</v>
-      </c>
-      <c r="K13" s="5" t="n">
+      <c r="K13" s="8" t="n">
         <v>31</v>
       </c>
-      <c r="L13" s="5" t="n">
+      <c r="L13" s="8" t="n">
         <v>91</v>
       </c>
-      <c r="M13" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="N13" s="5" t="n">
+      <c r="M13" s="8" t="n">
+        <v>40</v>
+      </c>
+      <c r="N13" s="8" t="n">
         <v>99</v>
       </c>
-      <c r="O13" s="5" t="n">
-        <f aca="false">ROUND(league!$H19*0.5, 0)</f>
-        <v>45</v>
+      <c r="O13" s="8" t="n">
+        <v>30</v>
       </c>
       <c r="P13" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q13" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="R13" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="S13" s="5" t="n">
-        <v>80</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="Q13" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="R13" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="S13" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="XEZ13" s="11"/>
+      <c r="XFA13" s="11"/>
+      <c r="XFB13" s="11"/>
+      <c r="XFC13" s="11"/>
+      <c r="XFD13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
@@ -1532,20 +1559,20 @@
       <c r="E14" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="7" t="s">
         <v>64</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>65</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="I14" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J14" s="3" t="n">
-        <f aca="false">league!$H2</f>
+        <f aca="false">League!$H2</f>
         <v>100</v>
       </c>
       <c r="K14" s="3" t="n">
@@ -1561,11 +1588,10 @@
         <v>95</v>
       </c>
       <c r="O14" s="3" t="n">
-        <f aca="false">ROUND(league!$H2*0.5, 0)</f>
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="P14" s="3" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q14" s="3" t="n">
         <v>80</v>
@@ -1594,21 +1620,21 @@
       <c r="E15" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="13" t="s">
         <v>68</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>65</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J15" s="5" t="n">
-        <f aca="false">league!$H16</f>
-        <v>91</v>
+        <f aca="false">League!$H16</f>
+        <v>34</v>
       </c>
       <c r="K15" s="5" t="n">
         <v>51</v>
@@ -1622,12 +1648,11 @@
       <c r="N15" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="O15" s="5" t="n">
-        <f aca="false">ROUND(league!$H16*0.5, 0)</f>
-        <v>46</v>
+      <c r="O15" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="P15" s="5" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="Q15" s="5" t="n">
         <v>80</v>
@@ -1639,67 +1664,71 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+    <row r="16" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="3" t="str">
+      <c r="C16" s="8" t="str">
         <f aca="false">A16&amp;" "&amp;B16</f>
         <v>Pedro Diniz</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D16" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="E16" s="3" t="n">
+      <c r="E16" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="3" t="n">
+      <c r="H16" s="8" t="n">
+        <v>34</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="J16" s="8" t="n">
+        <f aca="false">League!$H15</f>
+        <v>78</v>
+      </c>
+      <c r="K16" s="8" t="n">
+        <v>11</v>
+      </c>
+      <c r="L16" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="M16" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="N16" s="8" t="n">
         <v>91</v>
       </c>
-      <c r="I16" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="J16" s="3" t="n">
-        <f aca="false">league!$H15</f>
-        <v>96</v>
-      </c>
-      <c r="K16" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="L16" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="M16" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="N16" s="3" t="n">
-        <v>91</v>
-      </c>
-      <c r="O16" s="3" t="n">
-        <f aca="false">ROUND(league!$H15*0.5, 0)</f>
-        <v>48</v>
+      <c r="O16" s="8" t="n">
+        <v>35</v>
       </c>
       <c r="P16" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q16" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="R16" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="S16" s="3" t="n">
-        <v>80</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="Q16" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="R16" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="S16" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="XEZ16" s="11"/>
+      <c r="XFA16" s="11"/>
+      <c r="XFB16" s="11"/>
+      <c r="XFC16" s="11"/>
+      <c r="XFD16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
@@ -1718,21 +1747,21 @@
       <c r="E17" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="13" t="s">
         <v>74</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>72</v>
       </c>
       <c r="H17" s="3" t="n">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="I17" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J17" s="5" t="n">
-        <f aca="false">league!$H17</f>
-        <v>92</v>
+        <f aca="false">League!$H17</f>
+        <v>23</v>
       </c>
       <c r="K17" s="5" t="n">
         <v>2</v>
@@ -1746,12 +1775,11 @@
       <c r="N17" s="5" t="n">
         <v>91</v>
       </c>
-      <c r="O17" s="5" t="n">
-        <f aca="false">ROUND(league!$H17*0.5, 0)</f>
-        <v>46</v>
+      <c r="O17" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q17" s="5" t="n">
         <v>80</v>
@@ -1780,21 +1808,21 @@
       <c r="E18" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="7" t="s">
         <v>76</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>77</v>
       </c>
       <c r="H18" s="3" t="n">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="I18" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J18" s="3" t="n">
-        <f aca="false">league!$H8</f>
-        <v>88</v>
+        <f aca="false">League!$H8</f>
+        <v>70</v>
       </c>
       <c r="K18" s="3" t="n">
         <v>32</v>
@@ -1809,11 +1837,10 @@
         <v>100</v>
       </c>
       <c r="O18" s="3" t="n">
-        <f aca="false">ROUND(league!$H8*0.5, 0)</f>
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="P18" s="3" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q18" s="3" t="n">
         <v>80</v>
@@ -1842,7 +1869,7 @@
       <c r="E19" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="13" t="s">
         <v>80</v>
       </c>
       <c r="G19" s="5" t="s">
@@ -1852,11 +1879,11 @@
         <v>90</v>
       </c>
       <c r="I19" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J19" s="5" t="n">
-        <f aca="false">league!$H11</f>
-        <v>92</v>
+        <f aca="false">League!$H11</f>
+        <v>87</v>
       </c>
       <c r="K19" s="5" t="n">
         <v>85</v>
@@ -1870,12 +1897,11 @@
       <c r="N19" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="O19" s="5" t="n">
-        <f aca="false">ROUND(league!$H11*0.5, 0)</f>
-        <v>46</v>
+      <c r="O19" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="P19" s="5" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q19" s="5" t="n">
         <v>80</v>
@@ -1887,67 +1913,71 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+    <row r="20" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="3" t="str">
+      <c r="C20" s="8" t="str">
         <f aca="false">A20&amp;" "&amp;B20</f>
         <v>Marc Gene</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="8" t="n">
         <v>19</v>
       </c>
-      <c r="E20" s="3" t="n">
+      <c r="E20" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H20" s="3" t="n">
-        <v>94</v>
+      <c r="H20" s="8" t="n">
+        <v>40</v>
       </c>
       <c r="I20" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="J20" s="3" t="n">
-        <f aca="false">league!$H9</f>
+        <v>20</v>
+      </c>
+      <c r="J20" s="8" t="n">
+        <f aca="false">League!$H9</f>
+        <v>30</v>
+      </c>
+      <c r="K20" s="8" t="n">
+        <v>23</v>
+      </c>
+      <c r="L20" s="8" t="n">
         <v>93</v>
       </c>
-      <c r="K20" s="3" t="n">
-        <v>23</v>
-      </c>
-      <c r="L20" s="3" t="n">
-        <v>93</v>
-      </c>
-      <c r="M20" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="N20" s="3" t="n">
+      <c r="M20" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="N20" s="8" t="n">
         <v>92</v>
       </c>
-      <c r="O20" s="3" t="n">
-        <f aca="false">ROUND(league!$H9*0.5, 0)</f>
-        <v>47</v>
+      <c r="O20" s="8" t="n">
+        <v>40</v>
       </c>
       <c r="P20" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q20" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="R20" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="S20" s="3" t="n">
-        <v>80</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="Q20" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="R20" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="S20" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="XEZ20" s="11"/>
+      <c r="XFA20" s="11"/>
+      <c r="XFB20" s="11"/>
+      <c r="XFC20" s="11"/>
+      <c r="XFD20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
@@ -1966,21 +1996,21 @@
       <c r="E21" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="13" t="s">
         <v>87</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>84</v>
       </c>
       <c r="H21" s="3" t="n">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="I21" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J21" s="5" t="n">
-        <f aca="false">league!$H10</f>
-        <v>95</v>
+        <f aca="false">League!$H10</f>
+        <v>87</v>
       </c>
       <c r="K21" s="5" t="n">
         <v>43</v>
@@ -1994,12 +2024,11 @@
       <c r="N21" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="O21" s="5" t="n">
-        <f aca="false">ROUND(league!$H10*0.5, 0)</f>
-        <v>48</v>
+      <c r="O21" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="P21" s="5" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q21" s="5" t="n">
         <v>80</v>
@@ -2028,7 +2057,7 @@
       <c r="E22" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="13" t="s">
         <v>90</v>
       </c>
       <c r="G22" s="5" t="s">
@@ -2038,11 +2067,11 @@
         <v>97</v>
       </c>
       <c r="I22" s="3" t="n">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="J22" s="5" t="n">
-        <f aca="false">league!$H11</f>
-        <v>92</v>
+        <f aca="false">League!$H11</f>
+        <v>87</v>
       </c>
       <c r="K22" s="3" t="n">
         <v>79</v>
@@ -2056,12 +2085,11 @@
       <c r="N22" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="O22" s="5" t="n">
-        <f aca="false">ROUND(league!$H11*0.5, 0)</f>
-        <v>46</v>
+      <c r="O22" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="P22" s="3" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q22" s="5" t="n">
         <v>80</v>
@@ -2073,67 +2101,71 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+    <row r="23" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="5" t="str">
+      <c r="C23" s="8" t="str">
         <f aca="false">A23&amp;" "&amp;B23</f>
         <v>Ricardo Zonta</v>
       </c>
-      <c r="D23" s="5" t="n">
+      <c r="D23" s="8" t="n">
         <v>22</v>
       </c>
-      <c r="E23" s="5" t="n">
+      <c r="E23" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H23" s="3" t="n">
-        <v>91</v>
+      <c r="H23" s="8" t="n">
+        <v>16</v>
       </c>
       <c r="I23" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="J23" s="5" t="n">
-        <f aca="false">league!$H12</f>
+        <v>20</v>
+      </c>
+      <c r="J23" s="8" t="n">
+        <f aca="false">League!$H12</f>
         <v>92</v>
       </c>
-      <c r="K23" s="5" t="n">
+      <c r="K23" s="8" t="n">
         <v>54</v>
       </c>
-      <c r="L23" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="M23" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="N23" s="5" t="n">
+      <c r="L23" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="N23" s="8" t="n">
         <v>93</v>
       </c>
-      <c r="O23" s="5" t="n">
-        <f aca="false">ROUND(league!$H12*0.5, 0)</f>
-        <v>46</v>
+      <c r="O23" s="8" t="n">
+        <v>10</v>
       </c>
       <c r="P23" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q23" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="R23" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="S23" s="5" t="n">
-        <v>80</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="Q23" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="R23" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="S23" s="8" t="n">
+        <v>80</v>
+      </c>
+      <c r="XEZ23" s="11"/>
+      <c r="XFA23" s="11"/>
+      <c r="XFB23" s="11"/>
+      <c r="XFC23" s="11"/>
+      <c r="XFD23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
@@ -2152,21 +2184,21 @@
       <c r="E24" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>40</v>
+      <c r="G24" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H24" s="3" t="n">
         <v>100</v>
       </c>
       <c r="I24" s="3" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J24" s="5" t="n">
-        <f aca="false">league!$H13</f>
-        <v>90</v>
+        <f aca="false">League!$H13</f>
+        <v>20</v>
       </c>
       <c r="K24" s="3" t="n">
         <v>45</v>
@@ -2180,12 +2212,11 @@
       <c r="N24" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="O24" s="5" t="n">
-        <f aca="false">ROUND(league!$H13*0.5, 0)</f>
-        <v>45</v>
+      <c r="O24" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="P24" s="3" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q24" s="5" t="n">
         <v>80</v>
@@ -2214,21 +2245,21 @@
       <c r="E25" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="13" t="s">
         <v>100</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H25" s="3" t="n">
         <v>96</v>
       </c>
       <c r="I25" s="3" t="n">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="J25" s="5" t="n">
-        <f aca="false">league!$H14</f>
-        <v>91</v>
+        <f aca="false">League!$H14</f>
+        <v>68</v>
       </c>
       <c r="K25" s="5" t="n">
         <v>54</v>
@@ -2242,12 +2273,11 @@
       <c r="N25" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="O25" s="5" t="n">
-        <f aca="false">ROUND(league!$H14*0.5, 0)</f>
-        <v>46</v>
+      <c r="O25" s="3" t="n">
+        <v>95</v>
       </c>
       <c r="P25" s="5" t="n">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Q25" s="5" t="n">
         <v>80</v>
@@ -2287,289 +2317,289 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="14" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="0" t="s">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="A17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="A19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>135</v>
       </c>
     </row>

</xml_diff>